<commit_message>
updated Demo.xlsx and ReadExcel.java
</commit_message>
<xml_diff>
--- a/JavaInterview/Demo.xlsx
+++ b/JavaInterview/Demo.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nandi\ProgrammingInterviewQuestions\InterviewQuestions\JavaInterview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6353A9E4-D95F-4865-B738-395714E283DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C76D9F-7397-494D-AF02-B1012A154792}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D183265D-4ECE-446B-BA6A-97EEC3F0C3AE}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>Subhankar</t>
   </si>
@@ -49,12 +49,25 @@
   </si>
   <si>
     <t>Deb</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Write</t>
+  </si>
+  <si>
+    <t>10000</t>
+  </si>
+  <si>
+    <t>Demo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -476,16 +489,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38D4FB7D-86EA-43A0-8611-E9D5FCCED408}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.88671875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.77734375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -528,6 +541,38 @@
         <v>6</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>